<commit_message>
Modificato circuito per correggere impostazione corrente fotocoppie footprint SC-70 dei due operazionali sostituito con SOT-23-5
</commit_message>
<xml_diff>
--- a/ESECUTIVI/LP23-319-0.xlsx
+++ b/ESECUTIVI/LP23-319-0.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UTENTI\00.LAVORI IN CORSO\METALTRONICA\23-319-0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marco\Documents\Data\Progetti-GIT\HW\PCB-23-319\ESECUTIVI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{078E20FD-4D9A-4BD9-BC74-4D382C160E63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACCAE23E-E023-4D66-A614-869F52D1F842}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="23-319-0" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="66">
   <si>
     <t>Pos.</t>
   </si>
@@ -124,9 +124,6 @@
     <t>R6</t>
   </si>
   <si>
-    <t>1K7</t>
-  </si>
-  <si>
     <t>R7,R8</t>
   </si>
   <si>
@@ -202,7 +199,25 @@
     <t>ROHM</t>
   </si>
   <si>
-    <t>D: RPI-0352ETR-ND</t>
+    <t>VARI (0603YC104JAT2A)</t>
+  </si>
+  <si>
+    <t>MLCC, X7R, 16V 0603</t>
+  </si>
+  <si>
+    <t>F: 1740612</t>
+  </si>
+  <si>
+    <t>VARI (MC0603B103K160CT)</t>
+  </si>
+  <si>
+    <t>F:1759003</t>
+  </si>
+  <si>
+    <t>F: 3954435</t>
+  </si>
+  <si>
+    <t>1K8</t>
   </si>
 </sst>
 </file>
@@ -353,7 +368,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -536,6 +551,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -715,7 +736,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -734,6 +755,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Colore 1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1092,7 +1118,7 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1100,9 +1126,9 @@
     <col min="1" max="1" width="4" style="1" customWidth="1"/>
     <col min="2" max="2" width="4.140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="9.42578125" customWidth="1"/>
-    <col min="4" max="4" width="32.140625" customWidth="1"/>
+    <col min="4" max="4" width="54.7109375" customWidth="1"/>
     <col min="5" max="5" width="19.140625" customWidth="1"/>
-    <col min="6" max="6" width="18.5703125" customWidth="1"/>
+    <col min="6" max="6" width="25.5703125" customWidth="1"/>
     <col min="7" max="7" width="22.5703125" customWidth="1"/>
     <col min="8" max="8" width="10.42578125" customWidth="1"/>
     <col min="9" max="9" width="9.7109375" customWidth="1"/>
@@ -1111,11 +1137,11 @@
   <sheetData>
     <row r="1" spans="1:10" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B1" s="3"/>
       <c r="E1" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -1150,335 +1176,339 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="6">
+    <row r="4" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8">
         <v>1</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="8">
         <v>3</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="H4" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7" t="s">
+      <c r="I4" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" s="9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="8">
+        <v>2</v>
+      </c>
+      <c r="B5" s="8">
+        <v>3</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="H5" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="I5" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="J4" s="7" t="s">
+      <c r="J5" s="9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="8">
+        <v>3</v>
+      </c>
+      <c r="B6" s="8">
+        <v>1</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="8">
+        <v>4</v>
+      </c>
+      <c r="B7" s="8">
+        <v>2</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+    </row>
+    <row r="8" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="8">
+        <v>5</v>
+      </c>
+      <c r="B8" s="8">
+        <v>2</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="J8" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="8">
+        <v>6</v>
+      </c>
+      <c r="B9" s="8">
+        <v>1</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="J9" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="8">
+        <v>7</v>
+      </c>
+      <c r="B10" s="8">
+        <v>2</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="J10" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="8">
+        <v>8</v>
+      </c>
+      <c r="B11" s="8">
+        <v>1</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="I11" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="J11" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="8">
+        <v>9</v>
+      </c>
+      <c r="B12" s="8">
+        <v>2</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="I12" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="J12" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="8">
+        <v>10</v>
+      </c>
+      <c r="B13" s="8">
+        <v>1</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="I13" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="J13" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="8">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="6">
+      <c r="B14" s="8">
         <v>2</v>
       </c>
-      <c r="B5" s="6">
-        <v>3</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="I5" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="6">
-        <v>3</v>
-      </c>
-      <c r="B6" s="6">
-        <v>1</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="6">
-        <v>4</v>
-      </c>
-      <c r="B7" s="6">
-        <v>2</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="6">
-        <v>5</v>
-      </c>
-      <c r="B8" s="6">
-        <v>2</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="I8" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="J8" s="7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="6">
-        <v>6</v>
-      </c>
-      <c r="B9" s="6">
-        <v>1</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="I9" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="J9" s="7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="6">
-        <v>7</v>
-      </c>
-      <c r="B10" s="6">
-        <v>2</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="I10" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="J10" s="7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="6">
-        <v>8</v>
-      </c>
-      <c r="B11" s="6">
-        <v>1</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="I11" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="J11" s="7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="6">
-        <v>9</v>
-      </c>
-      <c r="B12" s="6">
-        <v>2</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="I12" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="J12" s="7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="6">
-        <v>10</v>
-      </c>
-      <c r="B13" s="6">
-        <v>1</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="G13" s="7" t="s">
+      <c r="C14" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="H14" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="H13" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="I13" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="J13" s="7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="6">
-        <v>11</v>
-      </c>
-      <c r="B14" s="6">
-        <v>2</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="F14" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="G14" s="7" t="s">
+      <c r="I14" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="H14" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="I14" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="J14" s="7"/>
+      <c r="J14" s="9"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
@@ -1488,28 +1518,28 @@
         <v>1</v>
       </c>
       <c r="C15" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="E15" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="F15" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="G15" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="F15" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="G15" s="7" t="s">
+      <c r="H15" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="H15" s="7" t="s">
+      <c r="I15" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="I15" s="7" t="s">
+      <c r="J15" s="7" t="s">
         <v>54</v>
-      </c>
-      <c r="J15" s="7" t="s">
-        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modificato C6 da 10nF a 100nF per possibile instabilità refererence
</commit_message>
<xml_diff>
--- a/ESECUTIVI/LP23-319-0.xlsx
+++ b/ESECUTIVI/LP23-319-0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Utenti\00.Lavori in corso\METALTRONICA\23-319-0 (Fotocoppie Lame Laterali)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marco\Documents\Data\Progetti-GIT\HW\PCB-23-319\ESECUTIVI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F9AD5943-064C-40D5-B620-C8F4E2036C7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DB5D8EC-64DB-41F6-A591-EEB488DF3C7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640"/>
+    <workbookView xWindow="-21720" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="23-319-0" sheetId="1" r:id="rId1"/>
@@ -52,9 +52,6 @@
     <t>Note</t>
   </si>
   <si>
-    <t>C1,C3,C4</t>
-  </si>
-  <si>
     <t>MLCC, X7R, 50V 0603</t>
   </si>
   <si>
@@ -64,9 +61,6 @@
     <t>VARI</t>
   </si>
   <si>
-    <t>C2,C5,C6</t>
-  </si>
-  <si>
     <t>10nF</t>
   </si>
   <si>
@@ -191,12 +185,18 @@
   </si>
   <si>
     <t>DATA 6/7/2023</t>
+  </si>
+  <si>
+    <t>C1,C3,C4,C6</t>
+  </si>
+  <si>
+    <t>C2,C5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1090,11 +1090,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:J14"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1112,11 +1112,11 @@
   <sheetData>
     <row r="1" spans="1:10" s="4" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B1" s="6"/>
       <c r="E1" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F1" s="5"/>
       <c r="I1" s="5"/>
@@ -1158,29 +1158,29 @@
         <v>1</v>
       </c>
       <c r="B3" s="12">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C3" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="E3" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="13" t="s">
-        <v>12</v>
-      </c>
       <c r="F3" s="14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G3" s="13"/>
       <c r="H3" s="13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I3" s="14" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="J3" s="13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -1188,29 +1188,29 @@
         <v>2</v>
       </c>
       <c r="B4" s="12">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>14</v>
+        <v>56</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G4" s="13"/>
       <c r="H4" s="13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I4" s="14" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="J4" s="13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -1221,28 +1221,28 @@
         <v>1</v>
       </c>
       <c r="C5" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="F5" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="G5" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="H5" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="G5" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="H5" s="13" t="s">
-        <v>20</v>
-      </c>
       <c r="I5" s="14" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="J5" s="13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -1253,16 +1253,16 @@
         <v>2</v>
       </c>
       <c r="C6" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>23</v>
-      </c>
       <c r="F6" s="14" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G6" s="13"/>
       <c r="H6" s="13"/>
@@ -1277,26 +1277,26 @@
         <v>2</v>
       </c>
       <c r="C7" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" s="13" t="s">
-        <v>26</v>
-      </c>
       <c r="F7" s="14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G7" s="13"/>
       <c r="H7" s="13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I7" s="14" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="J7" s="13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -1307,26 +1307,26 @@
         <v>2</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G8" s="13"/>
       <c r="H8" s="13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="J8" s="13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -1337,26 +1337,26 @@
         <v>1</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G9" s="13"/>
       <c r="H9" s="13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I9" s="14" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="J9" s="13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -1367,26 +1367,26 @@
         <v>2</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G10" s="13"/>
       <c r="H10" s="13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I10" s="14" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="J10" s="13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -1397,26 +1397,26 @@
         <v>1</v>
       </c>
       <c r="C11" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="E11" s="13" t="s">
-        <v>36</v>
-      </c>
       <c r="F11" s="14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G11" s="13"/>
       <c r="H11" s="13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I11" s="14" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="J11" s="13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -1427,26 +1427,26 @@
         <v>1</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G12" s="13"/>
       <c r="H12" s="13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I12" s="14" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="J12" s="13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -1457,25 +1457,25 @@
         <v>2</v>
       </c>
       <c r="C13" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="F13" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="G13" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="E13" s="13" t="s">
+      <c r="H13" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="F13" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="G13" s="13" t="s">
+      <c r="I13" s="14" t="s">
         <v>42</v>
-      </c>
-      <c r="H13" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="I13" s="14" t="s">
-        <v>44</v>
       </c>
       <c r="J13" s="13"/>
     </row>
@@ -1487,28 +1487,28 @@
         <v>1</v>
       </c>
       <c r="C14" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="E14" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="D14" s="13" t="s">
+      <c r="F14" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="G14" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="E14" s="13" t="s">
+      <c r="H14" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="F14" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="G14" s="13" t="s">
+      <c r="I14" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="H14" s="13" t="s">
+      <c r="J14" s="13" t="s">
         <v>49</v>
-      </c>
-      <c r="I14" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="J14" s="13" t="s">
-        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>